<commit_message>
Updated project with 6 hour forecasting model and structure updated
</commit_message>
<xml_diff>
--- a/outputs/error_output.xlsx
+++ b/outputs/error_output.xlsx
@@ -467,16 +467,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0204575799086758</v>
+        <v>0.105567857958438</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0008532765890410959</v>
+        <v>0.02204611458666362</v>
       </c>
       <c r="D2" t="n">
-        <v>0.02921089846343477</v>
+        <v>0.1484793406055658</v>
       </c>
       <c r="E2" t="n">
-        <v>0.983252836807158</v>
+        <v>0.5673587211986075</v>
       </c>
     </row>
     <row r="3">
@@ -486,16 +486,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.01870667597065709</v>
+        <v>0.0595534263883123</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00073963951497391</v>
+        <v>0.008399002011536651</v>
       </c>
       <c r="D3" t="n">
-        <v>0.02719631436378669</v>
+        <v>0.09164606926397144</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9852782967914673</v>
+        <v>0.8000169440541736</v>
       </c>
     </row>
     <row r="4">
@@ -505,16 +505,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.01982059139482336</v>
+        <v>0.06764041889202761</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0007963544318373755</v>
+        <v>0.00946676304975011</v>
       </c>
       <c r="D4" t="n">
-        <v>0.02821975251197954</v>
+        <v>0.09729729209875324</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9837609656313352</v>
+        <v>0.7768154607780005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Neural Network function transformed to class, updated main file,  model cleaned up using flake8
</commit_message>
<xml_diff>
--- a/outputs/error_output.xlsx
+++ b/outputs/error_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,85 +436,165 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Prediction Horizon</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Prediction Model Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Mean Absolute Error</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Mean Squared Error</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Root Mean Square Error</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>R Squared</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>persistence</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>0.105567857958438</v>
-      </c>
       <c r="C2" t="n">
-        <v>0.02204611458666362</v>
+        <v>0.02046225165562914</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1484793406055658</v>
+        <v>0.0008541031879424526</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5673587211986075</v>
+        <v>0.02922504384842652</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9832394036160876</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>random_forest</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>0.0595534263883123</v>
-      </c>
       <c r="C3" t="n">
-        <v>0.008399002011536651</v>
+        <v>0.005373401621674758</v>
       </c>
       <c r="D3" t="n">
-        <v>0.09164606926397144</v>
+        <v>0.0001075083204025303</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8000169440541736</v>
+        <v>0.01036862191433993</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9978876762261663</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>neural_network</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0.06764041889202761</v>
-      </c>
       <c r="C4" t="n">
-        <v>0.00946676304975011</v>
+        <v>0.009708198715866524</v>
       </c>
       <c r="D4" t="n">
-        <v>0.09729729209875324</v>
+        <v>0.0002432799561024466</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7768154607780005</v>
+        <v>0.01559743427947195</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9950598850805302</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>6</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>persistence</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.105567857958438</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.02204611458666362</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.1484793406055658</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.5673587211986075</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>random_forest</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0595534263883123</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.008399002011536651</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.09164606926397144</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.8000169440541736</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>neural_network</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.06599178062754969</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.009445472209663417</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.09718781924533247</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.776892828741772</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned files and updated neural network keras  functions to simplify them
</commit_message>
<xml_diff>
--- a/outputs/error_output.xlsx
+++ b/outputs/error_output.xlsx
@@ -475,16 +475,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.02046225165562914</v>
+        <v>0.02045644479963466</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0008541031879424526</v>
+        <v>0.0008532684964036991</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02922504384842652</v>
+        <v>0.029210759942249</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9832394036160876</v>
+        <v>0.9832547184925169</v>
       </c>
     </row>
     <row r="3">
@@ -497,16 +497,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.005373401621674758</v>
+        <v>0.005374860246620195</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0001075083204025303</v>
+        <v>0.0001076096118544995</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01036862191433993</v>
+        <v>0.010373505282907</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9978876762261663</v>
+        <v>0.9978856397616686</v>
       </c>
     </row>
     <row r="4">
@@ -519,16 +519,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.009708198715866524</v>
+        <v>0.01203881740834067</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0002432799561024466</v>
+        <v>0.0002962133632098551</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01559743427947195</v>
+        <v>0.01721085015941557</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9950598850805302</v>
+        <v>0.9941865463468429</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Updated error measures function, updated graph colours, updated README file
</commit_message>
<xml_diff>
--- a/outputs/error_output.xlsx
+++ b/outputs/error_output.xlsx
@@ -484,7 +484,7 @@
         <v>0.029210759942249</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9832547184925169</v>
+        <v>0.9832545374323554</v>
       </c>
     </row>
     <row r="3">
@@ -506,7 +506,7 @@
         <v>0.010373505282907</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9978856397616686</v>
+        <v>0.9978881527504846</v>
       </c>
     </row>
     <row r="4">
@@ -528,7 +528,7 @@
         <v>0.01721085015941557</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9941865463468429</v>
+        <v>0.9941867890276357</v>
       </c>
     </row>
     <row r="5">
@@ -550,7 +550,7 @@
         <v>0.1484793406055658</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5673587211986075</v>
+        <v>0.5673758213742874</v>
       </c>
     </row>
     <row r="6">
@@ -572,7 +572,7 @@
         <v>0.09164606926397144</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8000169440541736</v>
+        <v>0.8351813272024434</v>
       </c>
     </row>
     <row r="7">
@@ -594,7 +594,7 @@
         <v>0.09718781924533247</v>
       </c>
       <c r="F7" t="n">
-        <v>0.776892828741772</v>
+        <v>0.8146458125138485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>